<commit_message>
Update Power BI dashboard
</commit_message>
<xml_diff>
--- a/Dashboard FLF/Excel FLF/draft/draft final.xlsx
+++ b/Dashboard FLF/Excel FLF/draft/draft final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SMT6\MAGANG\MAGANG ITM\Intern\FLF Automation System\Dashboard FLF\Excel FLF\draft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955C3E44-A408-472C-88B2-055F694AC004}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B5DADF-AB37-4662-9B5F-24430C808E28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="2820" windowWidth="11496" windowHeight="6384" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="20">
   <si>
     <t>FLF</t>
   </si>
@@ -92,9 +92,6 @@
   </si>
   <si>
     <t>FC Sumber 1001</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -167,7 +164,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,12 +174,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -258,7 +249,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -339,10 +330,22 @@
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -779,8 +782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView zoomScale="119" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1094,99 +1097,64 @@
       <c r="M13" s="28"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="15">
+      <c r="B14" s="32">
         <v>45231</v>
       </c>
-      <c r="C14" s="20">
+      <c r="C14" s="33">
         <v>357290</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="20">
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="33">
         <v>418773</v>
       </c>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="21">
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="35">
         <v>52540</v>
       </c>
-      <c r="L14" s="18"/>
+      <c r="L14" s="34"/>
       <c r="M14" s="28"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="14">
+      <c r="B15" s="32">
         <v>45261</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="33">
         <v>167935</v>
       </c>
-      <c r="D15" s="20">
+      <c r="D15" s="33">
         <v>330795</v>
       </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="20">
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="33">
         <v>406070</v>
       </c>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="21">
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="35">
         <v>15000</v>
       </c>
-      <c r="L15" s="18"/>
+      <c r="L15" s="34"/>
       <c r="M15" s="28"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="31">
-        <f>SUM(C4:C15)</f>
-        <v>2075101</v>
-      </c>
-      <c r="D16" s="31">
-        <f t="shared" ref="D16:M16" si="0">SUM(D4:D15)</f>
-        <v>1304220</v>
-      </c>
-      <c r="E16" s="31">
-        <f t="shared" si="0"/>
-        <v>1183835.3360000001</v>
-      </c>
-      <c r="F16" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="31">
-        <f t="shared" si="0"/>
-        <v>3553840.77</v>
-      </c>
-      <c r="I16" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K16" s="31">
-        <f t="shared" si="0"/>
-        <v>590757.33400000003</v>
-      </c>
-      <c r="L16" s="31">
-        <f t="shared" si="0"/>
-        <v>286049.60600000003</v>
-      </c>
-      <c r="M16" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="B16" s="30"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="31"/>
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C18" s="19"/>
@@ -1211,7 +1179,7 @@
   <dimension ref="B2:N25"/>
   <sheetViews>
     <sheetView zoomScale="97" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1514,107 +1482,72 @@
       <c r="M13" s="28"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="14">
+      <c r="B14" s="32">
         <v>45597</v>
       </c>
-      <c r="C14" s="20">
+      <c r="C14" s="33">
         <v>331362</v>
       </c>
-      <c r="D14" s="20">
+      <c r="D14" s="33">
         <v>349798</v>
       </c>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="20">
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="33">
         <v>275671</v>
       </c>
-      <c r="I14" s="18"/>
-      <c r="J14" s="21">
+      <c r="I14" s="34"/>
+      <c r="J14" s="35">
         <v>61334</v>
       </c>
-      <c r="K14" s="21">
+      <c r="K14" s="35">
         <v>54400</v>
       </c>
-      <c r="L14" s="18"/>
+      <c r="L14" s="34"/>
       <c r="M14" s="28"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="14">
+      <c r="B15" s="32">
         <v>45627</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="33">
         <v>364621.5</v>
       </c>
-      <c r="D15" s="20">
+      <c r="D15" s="33">
         <v>314820.5</v>
       </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="20">
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="33">
         <v>427533</v>
       </c>
-      <c r="I15" s="18"/>
-      <c r="J15" s="21">
+      <c r="I15" s="34"/>
+      <c r="J15" s="35">
         <v>45060</v>
       </c>
-      <c r="K15" s="21">
+      <c r="K15" s="35">
         <v>144255</v>
       </c>
-      <c r="L15" s="21">
+      <c r="L15" s="35">
         <v>197580</v>
       </c>
       <c r="M15" s="28"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="31">
-        <f>SUM(C4:C15)</f>
-        <v>3133740.5</v>
-      </c>
-      <c r="D16" s="31">
-        <f t="shared" ref="D16:M16" si="0">SUM(D4:D15)</f>
-        <v>3959647.5</v>
-      </c>
-      <c r="E16" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="31">
-        <f t="shared" si="0"/>
-        <v>279814</v>
-      </c>
-      <c r="G16" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="31">
-        <f t="shared" si="0"/>
-        <v>3998991</v>
-      </c>
-      <c r="I16" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="31">
-        <f t="shared" si="0"/>
-        <v>248643.99999999997</v>
-      </c>
-      <c r="K16" s="31">
-        <f t="shared" si="0"/>
-        <v>518265</v>
-      </c>
-      <c r="L16" s="31">
-        <f t="shared" si="0"/>
-        <v>590935</v>
-      </c>
-      <c r="M16" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="B16" s="30"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="31"/>
     </row>
     <row r="20" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E20" s="23"/>
@@ -1632,7 +1565,7 @@
   <dimension ref="B2:M16"/>
   <sheetViews>
     <sheetView zoomScale="95" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1968,69 +1901,34 @@
       <c r="M14" s="28"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="14">
+      <c r="B15" s="32">
         <v>45992</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
       <c r="M15" s="28"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="31">
-        <f>SUM(C4:C15)</f>
-        <v>2713091</v>
-      </c>
-      <c r="D16" s="31">
-        <f t="shared" ref="D16:M16" si="0">SUM(D4:D15)</f>
-        <v>2902633.86</v>
-      </c>
-      <c r="E16" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="31">
-        <f t="shared" si="0"/>
-        <v>288995</v>
-      </c>
-      <c r="H16" s="31">
-        <f t="shared" si="0"/>
-        <v>3008758.14</v>
-      </c>
-      <c r="I16" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="31">
-        <f t="shared" si="0"/>
-        <v>319290</v>
-      </c>
-      <c r="K16" s="31">
-        <f t="shared" si="0"/>
-        <v>790625.00399999996</v>
-      </c>
-      <c r="L16" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M16" s="31">
-        <f t="shared" si="0"/>
-        <v>63065</v>
-      </c>
+      <c r="B16" s="30"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2042,8 +1940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCCD56A8-7428-4C2B-A9B9-94D659E4AB1C}">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>